<commit_message>
update notebooks up to POS features, WIP syntactic features
</commit_message>
<xml_diff>
--- a/comparison.xlsx
+++ b/comparison.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coolw\Dropbox\Programming\tts_proj\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coolw\Dropbox\Programming\tts_prosody\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11496" windowHeight="8976" xr2:uid="{1FC50A59-1A97-4F15-BC7E-C14F93769C94}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="8970" xr2:uid="{1FC50A59-1A97-4F15-BC7E-C14F93769C94}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -63,9 +62,6 @@
     <t>Old Score</t>
   </si>
   <si>
-    <t>Classification Report F1</t>
-  </si>
-  <si>
     <t>word_number_in_ipu</t>
   </si>
   <si>
@@ -100,6 +96,9 @@
   </si>
   <si>
     <t>syntactic</t>
+  </si>
+  <si>
+    <t>Classification Report F1 (ignore this!)</t>
   </si>
 </sst>
 </file>
@@ -478,26 +477,26 @@
   <dimension ref="A1:Y16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+      <selection activeCell="AA9" sqref="AA9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="8.88671875" style="1"/>
-    <col min="4" max="4" width="7.44140625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="3" width="8.85546875" style="1"/>
+    <col min="4" max="4" width="7.42578125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P1" s="2"/>
       <c r="Q1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="S1" s="2"/>
       <c r="T1" s="1" t="s">
@@ -505,10 +504,10 @@
       </c>
       <c r="V1" s="2"/>
       <c r="W1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -528,34 +527,34 @@
         <v>5</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>7</v>
@@ -585,7 +584,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -623,7 +622,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -661,7 +660,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -703,7 +702,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -749,7 +748,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -795,7 +794,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -836,7 +835,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -865,7 +864,7 @@
         <v>0.64900000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -894,7 +893,7 @@
         <v>0.67500000000000004</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -939,7 +938,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
@@ -986,7 +985,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
@@ -1036,7 +1035,7 @@
         <v>0.754</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -1086,7 +1085,7 @@
         <v>0.752</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="I16" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update OrganizedBigTable to order correctly, update files in info status
</commit_message>
<xml_diff>
--- a/comparison.xlsx
+++ b/comparison.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="24">
   <si>
     <t>word</t>
   </si>
@@ -66,9 +66,6 @@
   </si>
   <si>
     <t>Green means continuous</t>
-  </si>
-  <si>
-    <t>total_number_of_words_in_ipu</t>
   </si>
   <si>
     <t>Score</t>
@@ -105,10 +102,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.14999847407452621"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -149,17 +153,109 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -474,40 +570,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D8B1718-FE79-4AC3-B485-AAA055742648}">
-  <dimension ref="A1:Y16"/>
+  <dimension ref="A1:X16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA9" sqref="AA9"/>
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="8.85546875" style="1"/>
     <col min="4" max="4" width="7.42578125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="1"/>
+    <col min="5" max="15" width="8.85546875" style="1"/>
+    <col min="16" max="16" width="8.85546875" style="3"/>
+    <col min="17" max="17" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="8.85546875" style="1"/>
+    <col min="20" max="20" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="8.85546875" style="1"/>
+    <col min="23" max="23" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="S1" s="2"/>
-      <c r="T1" s="1" t="s">
+      <c r="O1" s="2"/>
+      <c r="P1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="V1" s="2"/>
-      <c r="W1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="V1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="W1"/>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -530,13 +632,13 @@
         <v>12</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="J2" t="s">
-        <v>14</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>18</v>
@@ -553,38 +655,35 @@
       <c r="O2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="P2" s="1" t="s">
-        <v>23</v>
+      <c r="P2" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="Q2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="S2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="W2" t="s">
         <v>8</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="W2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -603,64 +702,64 @@
       <c r="F3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="Q3" s="3">
+      <c r="P3" s="3">
         <v>0.63900000000000001</v>
       </c>
+      <c r="Q3" s="1">
+        <v>0.59</v>
+      </c>
       <c r="R3" s="1">
-        <v>0.59</v>
-      </c>
-      <c r="S3" s="1">
         <v>0.61699999999999999</v>
       </c>
+      <c r="V3" s="1">
+        <v>0.79</v>
+      </c>
       <c r="W3" s="1">
+        <v>0.62</v>
+      </c>
+      <c r="X3" s="1">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="P4" s="3">
+        <v>0.63300000000000001</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>0.61199999999999999</v>
+      </c>
+      <c r="R4" s="1">
+        <v>0.61099999999999999</v>
+      </c>
+      <c r="V4" s="1">
         <v>0.79</v>
       </c>
-      <c r="X3" s="1">
-        <v>0.62</v>
-      </c>
-      <c r="Y3" s="1">
+      <c r="W4" s="1">
         <v>0.82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q4" s="3">
-        <v>0.63300000000000001</v>
-      </c>
-      <c r="R4" s="1">
-        <v>0.61199999999999999</v>
-      </c>
-      <c r="S4" s="1">
-        <v>0.61099999999999999</v>
-      </c>
-      <c r="W4" s="1">
-        <v>0.79</v>
       </c>
       <c r="X4" s="1">
         <v>0.82</v>
       </c>
-      <c r="Y4" s="1">
-        <v>0.82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -674,35 +773,35 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
-      <c r="Q5" s="3">
+      <c r="P5" s="3">
         <v>0.63900000000000001</v>
       </c>
+      <c r="Q5" s="1">
+        <v>0.61399999999999999</v>
+      </c>
       <c r="R5" s="1">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="S5" s="1">
+        <v>0.63800000000000001</v>
+      </c>
+      <c r="T5" s="1">
+        <v>0.61599999999999999</v>
+      </c>
+      <c r="U5" s="1">
         <v>0.61399999999999999</v>
       </c>
-      <c r="S5" s="1">
-        <v>0.61499999999999999</v>
-      </c>
-      <c r="T5" s="1">
-        <v>0.63800000000000001</v>
-      </c>
-      <c r="U5" s="1">
-        <v>0.61599999999999999</v>
-      </c>
       <c r="V5" s="1">
-        <v>0.61399999999999999</v>
+        <v>0.79</v>
       </c>
       <c r="W5" s="1">
-        <v>0.79</v>
+        <v>0.82</v>
       </c>
       <c r="X5" s="1">
         <v>0.82</v>
       </c>
-      <c r="Y5" s="1">
-        <v>0.82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -720,35 +819,35 @@
       <c r="G6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="Q6" s="3">
+      <c r="P6" s="3">
         <v>0.63400000000000001</v>
       </c>
+      <c r="Q6" s="1">
+        <v>0.61399999999999999</v>
+      </c>
       <c r="R6" s="1">
+        <v>0.61699999999999999</v>
+      </c>
+      <c r="S6" s="1">
+        <v>0.63700000000000001</v>
+      </c>
+      <c r="T6" s="1">
         <v>0.61399999999999999</v>
       </c>
-      <c r="S6" s="3">
-        <v>0.61699999999999999</v>
-      </c>
-      <c r="T6" s="3">
-        <v>0.63700000000000001</v>
-      </c>
-      <c r="U6" s="3">
-        <v>0.61399999999999999</v>
-      </c>
-      <c r="V6" s="3">
+      <c r="U6" s="1">
         <v>0.61599999999999999</v>
       </c>
-      <c r="W6" s="3">
+      <c r="V6" s="1">
         <v>0.79</v>
+      </c>
+      <c r="W6" s="1">
+        <v>0.82</v>
       </c>
       <c r="X6" s="1">
         <v>0.82</v>
       </c>
-      <c r="Y6" s="1">
-        <v>0.82</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -766,105 +865,120 @@
       <c r="G7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="Q7" s="3">
+      <c r="P7" s="3">
         <v>0.63400000000000001</v>
       </c>
+      <c r="Q7" s="1">
+        <v>0.62</v>
+      </c>
       <c r="R7" s="1">
+        <v>0.61899999999999999</v>
+      </c>
+      <c r="S7" s="1">
+        <v>0.63300000000000001</v>
+      </c>
+      <c r="T7" s="1">
         <v>0.62</v>
       </c>
-      <c r="S7" s="3">
-        <v>0.61899999999999999</v>
-      </c>
-      <c r="T7" s="3">
-        <v>0.63300000000000001</v>
-      </c>
-      <c r="U7" s="3">
-        <v>0.62</v>
-      </c>
-      <c r="V7" s="3">
+      <c r="U7" s="1">
         <v>0.61699999999999999</v>
       </c>
-      <c r="W7" s="3">
+      <c r="V7" s="1">
         <v>0.79</v>
+      </c>
+      <c r="W7" s="1">
+        <v>0.82</v>
       </c>
       <c r="X7" s="1">
         <v>0.82</v>
       </c>
-      <c r="Y7" s="1">
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="P8" s="3">
+        <v>0.63900000000000001</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="R8" s="1">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="S8" s="1">
+        <v>0.63500000000000001</v>
+      </c>
+      <c r="T8" s="1">
+        <v>0.623</v>
+      </c>
+      <c r="U8" s="1">
+        <v>0.61899999999999999</v>
+      </c>
+      <c r="V8" s="1">
+        <v>0.79</v>
+      </c>
+      <c r="W8" s="1">
         <v>0.82</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q8" s="3">
-        <v>0.63900000000000001</v>
-      </c>
-      <c r="R8" s="1">
-        <v>0.61399999999999999</v>
-      </c>
-      <c r="S8" s="3">
-        <v>0.61499999999999999</v>
-      </c>
-      <c r="T8" s="3">
-        <v>0.63500000000000001</v>
-      </c>
-      <c r="U8" s="1">
-        <v>0.623</v>
-      </c>
-      <c r="V8" s="3">
-        <v>0.61899999999999999</v>
-      </c>
-      <c r="W8" s="3">
-        <v>0.79</v>
       </c>
       <c r="X8" s="1">
         <v>0.82</v>
       </c>
-      <c r="Y8" s="1">
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="P9" s="3">
+        <v>0.63900000000000001</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>0.626</v>
+      </c>
+      <c r="R9" s="1">
+        <v>0.627</v>
+      </c>
+      <c r="V9" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="W9" s="1">
+        <v>0.83</v>
+      </c>
+      <c r="X9" s="1">
         <v>0.82</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="T9" s="3">
-        <v>0.628</v>
-      </c>
-      <c r="U9" s="1">
-        <v>0.628</v>
-      </c>
-      <c r="V9" s="3">
-        <v>0.64900000000000002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -874,26 +988,50 @@
       <c r="C10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="T10" s="1">
-        <v>0.65600000000000003</v>
-      </c>
-      <c r="U10" s="1">
-        <v>0.66900000000000004</v>
+      <c r="D10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="P10" s="3">
+        <v>0.68600000000000005</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>0.745</v>
+      </c>
+      <c r="R10" s="1">
+        <v>0.74299999999999999</v>
       </c>
       <c r="V10" s="1">
-        <v>0.67500000000000004</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+        <v>0.83</v>
+      </c>
+      <c r="W10" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="X10" s="1">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -903,7 +1041,7 @@
       <c r="C11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" t="s">
         <v>6</v>
       </c>
       <c r="E11" s="3" t="s">
@@ -918,27 +1056,47 @@
       <c r="I11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J11" s="3"/>
+      <c r="J11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="P11" s="3">
+        <v>0.68799999999999994</v>
+      </c>
       <c r="Q11" s="1">
-        <v>0.63900000000000001</v>
+        <v>0.75</v>
       </c>
       <c r="R11" s="1">
-        <v>0.626</v>
-      </c>
-      <c r="S11" s="1">
-        <v>0.627</v>
+        <v>0.75</v>
+      </c>
+      <c r="S11" s="5">
+        <v>0.78600000000000003</v>
+      </c>
+      <c r="T11" s="5">
+        <v>0.85599999999999998</v>
+      </c>
+      <c r="U11" s="5">
+        <v>0.86</v>
+      </c>
+      <c r="V11" s="1">
+        <v>0.83</v>
       </c>
       <c r="W11" s="1">
-        <v>0.8</v>
+        <v>0.88</v>
       </c>
       <c r="X11" s="1">
-        <v>0.83</v>
-      </c>
-      <c r="Y11" s="1">
-        <v>0.82</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
@@ -963,6 +1121,9 @@
       <c r="I12" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="J12" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="K12" s="1" t="s">
         <v>6</v>
       </c>
@@ -975,17 +1136,35 @@
       <c r="N12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="T12" s="1">
-        <v>0.78600000000000003</v>
-      </c>
-      <c r="U12" s="1">
-        <v>0.85599999999999998</v>
+      <c r="P12" s="3">
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>0.752</v>
+      </c>
+      <c r="R12" s="1">
+        <v>0.754</v>
+      </c>
+      <c r="S12" s="5">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="T12" s="5">
+        <v>0.74399999999999999</v>
+      </c>
+      <c r="U12" s="5">
+        <v>0.754</v>
       </c>
       <c r="V12" s="1">
-        <v>0.86</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+        <v>0.84</v>
+      </c>
+      <c r="W12" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="X12" s="1">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
@@ -1010,10 +1189,7 @@
       <c r="I13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L13" s="1" t="s">
+      <c r="J13" s="1" t="s">
         <v>6</v>
       </c>
       <c r="M13" s="1" t="s">
@@ -1022,73 +1198,113 @@
       <c r="N13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="T13" s="1">
-        <v>0.71399999999999997</v>
-      </c>
-      <c r="U13" s="1">
-        <v>0.74399999999999999</v>
+      <c r="P13" s="3">
+        <v>0.69499999999999995</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>0.73299999999999998</v>
+      </c>
+      <c r="R13" s="1">
+        <v>0.73199999999999998</v>
       </c>
       <c r="V13" s="1">
-        <v>0.754</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="O14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="T14" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="W13" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="X13" s="1">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S15" s="5">
         <v>0.71299999999999997</v>
       </c>
-      <c r="U14" s="1">
+      <c r="T15" s="5">
         <v>0.745</v>
       </c>
-      <c r="V14" s="1">
+      <c r="U15" s="5">
         <v>0.752</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="I16" s="3"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="Q1:Q1048576">
+    <cfRule type="top10" dxfId="10" priority="11" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R1:R1048576">
+    <cfRule type="top10" dxfId="9" priority="10" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S1:S12 S14:S1048576">
+    <cfRule type="top10" dxfId="8" priority="9" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T1:T12 T14:T1048576">
+    <cfRule type="top10" dxfId="7" priority="8" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W3:W13">
+    <cfRule type="top10" dxfId="6" priority="5" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X1:X1048576">
+    <cfRule type="top10" dxfId="5" priority="4" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V1:V1048576">
+    <cfRule type="top10" dxfId="4" priority="3" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U1:U12 U14:U1048576">
+    <cfRule type="top10" dxfId="3" priority="2" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P14">
+    <cfRule type="top10" dxfId="2" priority="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P15:P1048576 P1:P13">
+    <cfRule type="top10" dxfId="1" priority="13" rank="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
run prosodic break detection on new dataset
</commit_message>
<xml_diff>
--- a/comparison.xlsx
+++ b/comparison.xlsx
@@ -1,18 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coolw\Dropbox\Programming\tts_prosody\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32311172-4E35-4845-BE8A-DD4ABF825458}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="8970" xr2:uid="{1FC50A59-1A97-4F15-BC7E-C14F93769C94}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="full_dataset" sheetId="2" r:id="rId1"/>
+    <sheet name="old" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="34">
   <si>
     <t>word</t>
   </si>
@@ -96,13 +98,43 @@
   </si>
   <si>
     <t>Classification Report F1 (ignore this!)</t>
+  </si>
+  <si>
+    <t>Stanford_PoS</t>
+  </si>
+  <si>
+    <t>RandomForestClassifier</t>
+  </si>
+  <si>
+    <t>Classification Report F1</t>
+  </si>
+  <si>
+    <t>syntactic_functions</t>
+  </si>
+  <si>
+    <t>Recent_Implicit_Mention_PoS</t>
+  </si>
+  <si>
+    <t>Recent_Explicit_Mention_PoS</t>
+  </si>
+  <si>
+    <t>Most_Recent_Mention_PoS</t>
+  </si>
+  <si>
+    <t>Recent_Implicit_Mention_Syntactic_Function</t>
+  </si>
+  <si>
+    <t>Recent_Explicit_Mention_Syntactic_Function</t>
+  </si>
+  <si>
+    <t>Most_Recent_Mention_Syntactic_Function</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,8 +149,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -129,6 +174,11 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -150,21 +200,91 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="26">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -569,11 +689,936 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E3431B5-E431-4926-B262-9A69677D0E6D}">
+  <dimension ref="A1:AC20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="19" max="19" width="9.140625" style="1"/>
+    <col min="21" max="23" width="9.140625" style="1"/>
+    <col min="26" max="26" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="V3" s="3">
+        <v>0.52200000000000002</v>
+      </c>
+      <c r="W3" s="1">
+        <v>0.499</v>
+      </c>
+      <c r="X3" s="1">
+        <v>0.51</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>0.49299999999999999</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="AA3" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="AB3" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="AC3" s="1">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="V4" s="3">
+        <v>0.52600000000000002</v>
+      </c>
+      <c r="W4" s="1">
+        <v>0.498</v>
+      </c>
+      <c r="X4" s="1">
+        <v>0.51</v>
+      </c>
+      <c r="Y4" s="1">
+        <v>0.48899999999999999</v>
+      </c>
+      <c r="Z4" s="1">
+        <v>0.78</v>
+      </c>
+      <c r="AA4" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="AB4" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="AC4" s="1">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="V5" s="3">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="W5" s="1">
+        <v>0.52300000000000002</v>
+      </c>
+      <c r="X5" s="1">
+        <v>0.53400000000000003</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>0.51</v>
+      </c>
+      <c r="Z5" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="AA5" s="1">
+        <v>0.86</v>
+      </c>
+      <c r="AB5" s="1">
+        <v>0.86</v>
+      </c>
+      <c r="AC5" s="1">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="V6" s="3">
+        <v>0.54900000000000004</v>
+      </c>
+      <c r="W6" s="1">
+        <v>0.52400000000000002</v>
+      </c>
+      <c r="X6" s="1">
+        <v>0.53400000000000003</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>0.505</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="AA6" s="1">
+        <v>0.86</v>
+      </c>
+      <c r="AB6" s="1">
+        <v>0.86</v>
+      </c>
+      <c r="AC6" s="1">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="V7" s="3">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="W7" s="1">
+        <v>0.52600000000000002</v>
+      </c>
+      <c r="X7" s="1">
+        <v>0.53400000000000003</v>
+      </c>
+      <c r="Y7" s="1">
+        <v>0.503</v>
+      </c>
+      <c r="Z7" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="AA7" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="AB7" s="1">
+        <v>0.86</v>
+      </c>
+      <c r="AC7" s="1">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="V8" s="3">
+        <v>0.54700000000000004</v>
+      </c>
+      <c r="W8" s="1">
+        <v>0.52400000000000002</v>
+      </c>
+      <c r="X8" s="1">
+        <v>0.53400000000000003</v>
+      </c>
+      <c r="Y8" s="1">
+        <v>0.50600000000000001</v>
+      </c>
+      <c r="Z8" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="AA8" s="1">
+        <v>0.86</v>
+      </c>
+      <c r="AB8" s="1">
+        <v>0.86</v>
+      </c>
+      <c r="AC8" s="1">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="R9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="V9" s="3">
+        <v>0.56699999999999995</v>
+      </c>
+      <c r="W9" s="1">
+        <v>0.624</v>
+      </c>
+      <c r="X9" s="1">
+        <v>0.626</v>
+      </c>
+      <c r="Y9" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="Z9" s="1">
+        <v>0.83</v>
+      </c>
+      <c r="AA9" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="AB9" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="AC9" s="1">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="R10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="V10" s="3">
+        <v>0.56899999999999995</v>
+      </c>
+      <c r="W10" s="1">
+        <v>0.624</v>
+      </c>
+      <c r="X10" s="1">
+        <v>0.627</v>
+      </c>
+      <c r="Y10" s="1">
+        <v>0.59899999999999998</v>
+      </c>
+      <c r="Z10" s="1">
+        <v>0.83</v>
+      </c>
+      <c r="AA10" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="AB10" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="AC10" s="1">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="R11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="S11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="T11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="V11" s="3">
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="W11" s="1">
+        <v>0.626</v>
+      </c>
+      <c r="X11" s="1">
+        <v>0.629</v>
+      </c>
+      <c r="Y11" s="1">
+        <v>0.59299999999999997</v>
+      </c>
+      <c r="Z11" s="1">
+        <v>0.83</v>
+      </c>
+      <c r="AA11" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="AB11" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="AC11" s="1">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="1"/>
+      <c r="W12" s="5"/>
+      <c r="X12" s="1"/>
+      <c r="Y12" s="1"/>
+      <c r="AA12" s="1"/>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="1"/>
+      <c r="X13" s="1"/>
+      <c r="Y13" s="1"/>
+      <c r="AA13" s="1"/>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="X14" s="1"/>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="T15" s="5"/>
+      <c r="X15" s="1"/>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="I20" s="1"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="W12 T14:T15">
+    <cfRule type="top10" dxfId="25" priority="19" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P14">
+    <cfRule type="top10" dxfId="24" priority="14" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC2">
+    <cfRule type="top10" dxfId="23" priority="9" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB2">
+    <cfRule type="top10" dxfId="22" priority="7" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB5">
+    <cfRule type="top10" dxfId="21" priority="5" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA2">
+    <cfRule type="top10" dxfId="20" priority="3" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA5">
+    <cfRule type="top10" dxfId="19" priority="2" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X14:X15 AA12:AA13">
+    <cfRule type="top10" dxfId="18" priority="33" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z1:Z1048576">
+    <cfRule type="top10" dxfId="17" priority="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q14:Q15 T12:T13 W1:W11">
+    <cfRule type="top10" dxfId="16" priority="34" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R14:R15 U12:U13 X1:X11">
+    <cfRule type="top10" dxfId="15" priority="38" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S12:S13 P15 V1:V11">
+    <cfRule type="top10" dxfId="14" priority="42" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S14:S1048576 V12:V13 Y1:Y11">
+    <cfRule type="top10" dxfId="13" priority="46" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W14:W1048576 AC1 AC3:AC11">
+    <cfRule type="top10" dxfId="12" priority="50" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V14:V1048576 AB1 AB3:AB4 Y12:Y13 AB6:AB11">
+    <cfRule type="top10" dxfId="11" priority="54" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U14:U1048576 AA1 AA3:AA4 X12:X13 AA6:AA11">
+    <cfRule type="top10" dxfId="10" priority="60" rank="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D8B1718-FE79-4AC3-B485-AAA055742648}">
   <dimension ref="A1:X16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L2" sqref="J2:L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1275,34 +2320,34 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="Q1:Q1048576">
-    <cfRule type="top10" dxfId="10" priority="11" rank="1"/>
+    <cfRule type="top10" dxfId="9" priority="11" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:R1048576">
-    <cfRule type="top10" dxfId="9" priority="10" rank="1"/>
+    <cfRule type="top10" dxfId="8" priority="10" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1:S12 S14:S1048576">
-    <cfRule type="top10" dxfId="8" priority="9" rank="1"/>
+    <cfRule type="top10" dxfId="7" priority="9" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1:T12 T14:T1048576">
-    <cfRule type="top10" dxfId="7" priority="8" rank="1"/>
+    <cfRule type="top10" dxfId="6" priority="8" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="W3:W13">
-    <cfRule type="top10" dxfId="6" priority="5" rank="1"/>
+    <cfRule type="top10" dxfId="5" priority="5" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="X1:X1048576">
-    <cfRule type="top10" dxfId="5" priority="4" rank="1"/>
+    <cfRule type="top10" dxfId="4" priority="4" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V1:V1048576">
-    <cfRule type="top10" dxfId="4" priority="3" rank="1"/>
+    <cfRule type="top10" dxfId="3" priority="3" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:U12 U14:U1048576">
-    <cfRule type="top10" dxfId="3" priority="2" rank="1"/>
+    <cfRule type="top10" dxfId="2" priority="2" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P14">
-    <cfRule type="top10" dxfId="2" priority="1" rank="1"/>
+    <cfRule type="top10" dxfId="1" priority="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P15:P1048576 P1:P13">
-    <cfRule type="top10" dxfId="1" priority="13" rank="1"/>
+    <cfRule type="top10" dxfId="0" priority="13" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update a few more files with config files
</commit_message>
<xml_diff>
--- a/comparison.xlsx
+++ b/comparison.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coolw\Dropbox\Programming\tts_prosody\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32311172-4E35-4845-BE8A-DD4ABF825458}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{290AED98-2EBD-4773-8081-E2D16E3ECEDE}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="8970" xr2:uid="{1FC50A59-1A97-4F15-BC7E-C14F93769C94}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="8970" activeTab="1" xr2:uid="{1FC50A59-1A97-4F15-BC7E-C14F93769C94}"/>
   </bookViews>
   <sheets>
     <sheet name="full_dataset" sheetId="2" r:id="rId1"/>
-    <sheet name="old" sheetId="1" r:id="rId2"/>
+    <sheet name="without autogenerated" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="32">
   <si>
     <t>word</t>
   </si>
@@ -61,9 +61,6 @@
     <t>Features</t>
   </si>
   <si>
-    <t>Old Score</t>
-  </si>
-  <si>
     <t>word_number_in_ipu</t>
   </si>
   <si>
@@ -95,9 +92,6 @@
   </si>
   <si>
     <t>syntactic</t>
-  </si>
-  <si>
-    <t>Classification Report F1 (ignore this!)</t>
   </si>
   <si>
     <t>Stanford_PoS</t>
@@ -163,7 +157,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -179,6 +173,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFBDBD"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -204,7 +204,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -213,6 +213,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -379,6 +381,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFBDBD"/>
+      <color rgb="FFFFB9B9"/>
       <color rgb="FF9999FF"/>
     </mruColors>
   </colors>
@@ -692,7 +696,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E3431B5-E431-4926-B262-9A69677D0E6D}">
   <dimension ref="A1:AC20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
@@ -708,7 +712,7 @@
         <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -724,12 +728,12 @@
       <c r="N1" s="1"/>
       <c r="U1" s="2"/>
       <c r="V1" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
       <c r="Z1" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
@@ -740,7 +744,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
@@ -753,46 +757,46 @@
         <v>5</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="T2" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="V2" s="3" t="s">
         <v>7</v>
@@ -804,7 +808,7 @@
         <v>9</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="Z2" s="1" t="s">
         <v>7</v>
@@ -816,7 +820,7 @@
         <v>9</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
@@ -1617,51 +1621,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D8B1718-FE79-4AC3-B485-AAA055742648}">
   <dimension ref="A1:X16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="J2:L2"/>
+    <sheetView tabSelected="1" topLeftCell="O2" workbookViewId="0">
+      <selection activeCell="Y17" sqref="Y17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="8.85546875" style="1"/>
+    <col min="2" max="3" width="8.85546875" style="8"/>
     <col min="4" max="4" width="7.42578125" style="1" customWidth="1"/>
-    <col min="5" max="15" width="8.85546875" style="1"/>
-    <col min="16" max="16" width="8.85546875" style="3"/>
-    <col min="17" max="17" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="8.85546875" style="1"/>
-    <col min="20" max="20" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="8.85546875" style="1"/>
-    <col min="23" max="23" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="8.85546875" style="1"/>
+    <col min="5" max="16" width="8.85546875" style="1"/>
+    <col min="17" max="17" width="8.85546875" style="3"/>
+    <col min="18" max="18" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="8.85546875" style="1"/>
+    <col min="21" max="21" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2"/>
-      <c r="P1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="W1"/>
+      <c r="U1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="V1"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="8" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -1674,68 +1674,68 @@
         <v>5</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="U2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="V2" t="s">
         <v>8</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="V2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="W2" t="s">
-        <v>8</v>
-      </c>
       <c r="X2" s="1" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -1747,22 +1747,22 @@
       <c r="F3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="3">
+      <c r="Q3" s="3">
         <v>0.63900000000000001</v>
       </c>
-      <c r="Q3" s="1">
+      <c r="R3" s="1">
         <v>0.59</v>
       </c>
-      <c r="R3" s="1">
+      <c r="S3" s="1">
         <v>0.61699999999999999</v>
       </c>
+      <c r="U3" s="1">
+        <v>0.79</v>
+      </c>
       <c r="V3" s="1">
-        <v>0.79</v>
+        <v>0.62</v>
       </c>
       <c r="W3" s="1">
-        <v>0.62</v>
-      </c>
-      <c r="X3" s="1">
         <v>0.82</v>
       </c>
     </row>
@@ -1770,10 +1770,10 @@
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -1785,75 +1785,66 @@
       <c r="F4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="3">
+      <c r="Q4" s="3">
         <v>0.63300000000000001</v>
       </c>
-      <c r="Q4" s="1">
+      <c r="R4" s="1">
         <v>0.61199999999999999</v>
       </c>
-      <c r="R4" s="1">
+      <c r="S4" s="1">
         <v>0.61099999999999999</v>
       </c>
+      <c r="U4" s="1">
+        <v>0.79</v>
+      </c>
       <c r="V4" s="1">
-        <v>0.79</v>
+        <v>0.82</v>
       </c>
       <c r="W4" s="1">
         <v>0.82</v>
       </c>
-      <c r="X4" s="1">
-        <v>0.82</v>
-      </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="B5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
-      <c r="P5" s="3">
+      <c r="Q5" s="3">
         <v>0.63900000000000001</v>
       </c>
-      <c r="Q5" s="1">
+      <c r="R5" s="1">
         <v>0.61399999999999999</v>
       </c>
-      <c r="R5" s="1">
+      <c r="S5" s="1">
         <v>0.61499999999999999</v>
       </c>
-      <c r="S5" s="1">
-        <v>0.63800000000000001</v>
-      </c>
-      <c r="T5" s="1">
-        <v>0.61599999999999999</v>
-      </c>
       <c r="U5" s="1">
-        <v>0.61399999999999999</v>
+        <v>0.79</v>
       </c>
       <c r="V5" s="1">
-        <v>0.79</v>
+        <v>0.82</v>
       </c>
       <c r="W5" s="1">
         <v>0.82</v>
       </c>
-      <c r="X5" s="1">
-        <v>0.82</v>
-      </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="B6" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="4" t="s">
@@ -1864,42 +1855,33 @@
       <c r="G6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="P6" s="3">
+      <c r="Q6" s="3">
         <v>0.63400000000000001</v>
       </c>
-      <c r="Q6" s="1">
+      <c r="R6" s="1">
         <v>0.61399999999999999</v>
       </c>
-      <c r="R6" s="1">
+      <c r="S6" s="1">
         <v>0.61699999999999999</v>
       </c>
-      <c r="S6" s="1">
-        <v>0.63700000000000001</v>
-      </c>
-      <c r="T6" s="1">
-        <v>0.61399999999999999</v>
-      </c>
       <c r="U6" s="1">
-        <v>0.61599999999999999</v>
+        <v>0.79</v>
       </c>
       <c r="V6" s="1">
-        <v>0.79</v>
+        <v>0.82</v>
       </c>
       <c r="W6" s="1">
         <v>0.82</v>
       </c>
-      <c r="X6" s="1">
-        <v>0.82</v>
-      </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="B7" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="4" t="s">
@@ -1910,83 +1892,65 @@
       <c r="G7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="P7" s="3">
+      <c r="Q7" s="3">
         <v>0.63400000000000001</v>
       </c>
-      <c r="Q7" s="1">
+      <c r="R7" s="1">
         <v>0.62</v>
       </c>
-      <c r="R7" s="1">
+      <c r="S7" s="1">
         <v>0.61899999999999999</v>
       </c>
-      <c r="S7" s="1">
-        <v>0.63300000000000001</v>
-      </c>
-      <c r="T7" s="1">
-        <v>0.62</v>
-      </c>
       <c r="U7" s="1">
-        <v>0.61699999999999999</v>
+        <v>0.79</v>
       </c>
       <c r="V7" s="1">
-        <v>0.79</v>
+        <v>0.82</v>
       </c>
       <c r="W7" s="1">
         <v>0.82</v>
       </c>
-      <c r="X7" s="1">
-        <v>0.82</v>
-      </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="B8" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="P8" s="3">
+      <c r="Q8" s="3">
         <v>0.63900000000000001</v>
       </c>
-      <c r="Q8" s="1">
+      <c r="R8" s="1">
         <v>0.61399999999999999</v>
       </c>
-      <c r="R8" s="1">
+      <c r="S8" s="1">
         <v>0.61499999999999999</v>
       </c>
-      <c r="S8" s="1">
-        <v>0.63500000000000001</v>
-      </c>
-      <c r="T8" s="1">
-        <v>0.623</v>
-      </c>
       <c r="U8" s="1">
-        <v>0.61899999999999999</v>
+        <v>0.79</v>
       </c>
       <c r="V8" s="1">
-        <v>0.79</v>
+        <v>0.82</v>
       </c>
       <c r="W8" s="1">
         <v>0.82</v>
       </c>
-      <c r="X8" s="1">
-        <v>0.82</v>
-      </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="B9" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="4" t="s">
@@ -2004,22 +1968,22 @@
       <c r="I9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="P9" s="3">
+      <c r="Q9" s="3">
         <v>0.63900000000000001</v>
       </c>
-      <c r="Q9" s="1">
+      <c r="R9" s="1">
         <v>0.626</v>
       </c>
-      <c r="R9" s="1">
+      <c r="S9" s="1">
         <v>0.627</v>
       </c>
+      <c r="U9" s="1">
+        <v>0.8</v>
+      </c>
       <c r="V9" s="1">
-        <v>0.8</v>
+        <v>0.83</v>
       </c>
       <c r="W9" s="1">
-        <v>0.83</v>
-      </c>
-      <c r="X9" s="1">
         <v>0.82</v>
       </c>
     </row>
@@ -2027,10 +1991,10 @@
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="B10" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="4" t="s">
@@ -2057,33 +2021,33 @@
       <c r="L10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="P10" s="3">
+      <c r="Q10" s="3">
         <v>0.68600000000000005</v>
       </c>
-      <c r="Q10" s="1">
+      <c r="R10" s="1">
         <v>0.745</v>
       </c>
-      <c r="R10" s="1">
+      <c r="S10" s="1">
         <v>0.74299999999999999</v>
       </c>
+      <c r="U10" s="1">
+        <v>0.83</v>
+      </c>
       <c r="V10" s="1">
-        <v>0.83</v>
+        <v>0.88</v>
       </c>
       <c r="W10" s="1">
         <v>0.88</v>
       </c>
-      <c r="X10" s="1">
-        <v>0.88</v>
-      </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="3" t="s">
+      <c r="B11" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D11" t="s">
@@ -2113,42 +2077,33 @@
       <c r="M11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="P11" s="3">
+      <c r="Q11" s="3">
         <v>0.68799999999999994</v>
-      </c>
-      <c r="Q11" s="1">
-        <v>0.75</v>
       </c>
       <c r="R11" s="1">
         <v>0.75</v>
       </c>
-      <c r="S11" s="5">
-        <v>0.78600000000000003</v>
-      </c>
-      <c r="T11" s="5">
-        <v>0.85599999999999998</v>
-      </c>
-      <c r="U11" s="5">
-        <v>0.86</v>
+      <c r="S11" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="U11" s="1">
+        <v>0.83</v>
       </c>
       <c r="V11" s="1">
-        <v>0.83</v>
+        <v>0.88</v>
       </c>
       <c r="W11" s="1">
         <v>0.88</v>
       </c>
-      <c r="X11" s="1">
-        <v>0.88</v>
-      </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="3" t="s">
+      <c r="B12" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="4" t="s">
@@ -2181,42 +2136,33 @@
       <c r="N12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="P12" s="3">
+      <c r="Q12" s="3">
         <v>0.70499999999999996</v>
       </c>
-      <c r="Q12" s="1">
+      <c r="R12" s="1">
         <v>0.752</v>
       </c>
-      <c r="R12" s="1">
+      <c r="S12" s="1">
         <v>0.754</v>
       </c>
-      <c r="S12" s="5">
-        <v>0.71399999999999997</v>
-      </c>
-      <c r="T12" s="5">
-        <v>0.74399999999999999</v>
-      </c>
-      <c r="U12" s="5">
-        <v>0.754</v>
+      <c r="U12" s="1">
+        <v>0.84</v>
       </c>
       <c r="V12" s="1">
-        <v>0.84</v>
+        <v>0.88</v>
       </c>
       <c r="W12" s="1">
         <v>0.88</v>
       </c>
-      <c r="X12" s="1">
-        <v>0.88</v>
-      </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="3" t="s">
+      <c r="B13" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D13" s="4" t="s">
@@ -2243,22 +2189,22 @@
       <c r="N13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="P13" s="3">
+      <c r="Q13" s="3">
         <v>0.69499999999999995</v>
       </c>
-      <c r="Q13" s="1">
+      <c r="R13" s="1">
         <v>0.73299999999999998</v>
       </c>
-      <c r="R13" s="1">
+      <c r="S13" s="1">
         <v>0.73199999999999998</v>
       </c>
+      <c r="U13" s="1">
+        <v>0.84</v>
+      </c>
       <c r="V13" s="1">
-        <v>0.84</v>
+        <v>0.88</v>
       </c>
       <c r="W13" s="1">
-        <v>0.88</v>
-      </c>
-      <c r="X13" s="1">
         <v>0.87</v>
       </c>
     </row>
@@ -2266,13 +2212,9 @@
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="4" t="s">
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E15" s="3" t="s">
@@ -2305,49 +2247,61 @@
       <c r="O15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="S15" s="5">
-        <v>0.71299999999999997</v>
-      </c>
-      <c r="T15" s="5">
-        <v>0.745</v>
-      </c>
-      <c r="U15" s="5">
-        <v>0.752</v>
+      <c r="Q15" s="3">
+        <v>0.70099999999999996</v>
+      </c>
+      <c r="R15" s="1">
+        <v>0.747</v>
+      </c>
+      <c r="S15" s="1">
+        <v>0.746</v>
+      </c>
+      <c r="T15" s="1">
+        <v>0.73299999999999998</v>
+      </c>
+      <c r="U15" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="V15" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="W15" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="X15" s="1">
+        <v>0.88</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="I16" s="3"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="Q1:Q1048576">
-    <cfRule type="top10" dxfId="9" priority="11" rank="1"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="R1:R1048576">
-    <cfRule type="top10" dxfId="8" priority="10" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S1:S12 S14:S1048576">
-    <cfRule type="top10" dxfId="7" priority="9" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T1:T12 T14:T1048576">
-    <cfRule type="top10" dxfId="6" priority="8" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="W3:W13">
-    <cfRule type="top10" dxfId="5" priority="5" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X1:X1048576">
+    <cfRule type="top10" dxfId="9" priority="14" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V3:V13">
+    <cfRule type="top10" dxfId="7" priority="8" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V14:V1048576 W1:W13 W15">
+    <cfRule type="top10" dxfId="6" priority="7" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U1:U13 U15">
+    <cfRule type="top10" dxfId="5" priority="6" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q14">
     <cfRule type="top10" dxfId="4" priority="4" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V1:V1048576">
-    <cfRule type="top10" dxfId="3" priority="3" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="U1:U12 U14:U1048576">
-    <cfRule type="top10" dxfId="2" priority="2" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P14">
-    <cfRule type="top10" dxfId="1" priority="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P15:P1048576 P1:P13">
-    <cfRule type="top10" dxfId="0" priority="13" rank="1"/>
+  <conditionalFormatting sqref="Q15:Q1048576 Q1:Q13">
+    <cfRule type="top10" dxfId="3" priority="16" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S1:S1048576">
+    <cfRule type="top10" dxfId="2" priority="3" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T1:T1048576">
+    <cfRule type="top10" dxfId="1" priority="2" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X1:X13 X15">
+    <cfRule type="top10" dxfId="0" priority="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add pitch accent gold standard to Classifier_main, update comparison
</commit_message>
<xml_diff>
--- a/comparison.xlsx
+++ b/comparison.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coolw\Dropbox\Programming\tts_prosody\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{290AED98-2EBD-4773-8081-E2D16E3ECEDE}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A907D6E8-51AA-460D-9281-D9BF72A5C8C7}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="8970" activeTab="1" xr2:uid="{1FC50A59-1A97-4F15-BC7E-C14F93769C94}"/>
   </bookViews>
   <sheets>
-    <sheet name="full_dataset" sheetId="2" r:id="rId1"/>
-    <sheet name="without autogenerated" sheetId="1" r:id="rId2"/>
+    <sheet name="final numbers" sheetId="3" r:id="rId1"/>
+    <sheet name="table for final report" sheetId="4" r:id="rId2"/>
+    <sheet name="full_dataset OLD" sheetId="2" r:id="rId3"/>
+    <sheet name="without autogenerated OLD" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="63">
   <si>
     <t>word</t>
   </si>
@@ -122,13 +124,106 @@
   </si>
   <si>
     <t>Most_Recent_Mention_Syntactic_Function</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Precision</t>
+  </si>
+  <si>
+    <t>Recall</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>F.25</t>
+  </si>
+  <si>
+    <t>RandomForest</t>
+  </si>
+  <si>
+    <t>GridSearchCV done for best F.25 score</t>
+  </si>
+  <si>
+    <t>Most_Recent_Mention_Syntactic_Function,Recent_Explicit_Mention_Syntactic_Function, Recent_Implicit_Mention_Syntactic_Function, Most_Recent_Mention_PoS, Recent_Explicit_Mention_PoS, Recent_Implicit_Mention_PoS,</t>
+  </si>
+  <si>
+    <t>KEY:</t>
+  </si>
+  <si>
+    <t>task and turn</t>
+  </si>
+  <si>
+    <t>word_number_in_turn, word_number_in_task, total_number_of_words_in_turn, total_number_of_words_in_task</t>
+  </si>
+  <si>
+    <t>syntactic_function</t>
+  </si>
+  <si>
+    <t>basic mention</t>
+  </si>
+  <si>
+    <t>more mention</t>
+  </si>
+  <si>
+    <t>mentioned, Number_Of_Coref_Mentions, time_between_mentions (generated by functions in a notebook cell)</t>
+  </si>
+  <si>
+    <t>bigram features</t>
+  </si>
+  <si>
+    <t>pos_bigram, word_bigram, dist_end_turn (for bigram features both _left and _right)</t>
+  </si>
+  <si>
+    <t>spanning tree</t>
+  </si>
+  <si>
+    <t>tree_depth, tree_width, word_depth, constituent_width, constituent_label, constituent_forward_position, constituent_backward_position</t>
+  </si>
+  <si>
+    <t>colored cells explained below</t>
+  </si>
+  <si>
+    <t>accent_gold_labels</t>
+  </si>
+  <si>
+    <t>accent-1, accent0, accent1</t>
+  </si>
+  <si>
+    <t>Y (no word_bigram)</t>
+  </si>
+  <si>
+    <t>Baseline</t>
+  </si>
+  <si>
+    <t>NOTES:</t>
+  </si>
+  <si>
+    <t>row 10 uses accent_gold_labels, which are not linguistic-only features. In the future this should be replaced with pitch accent ratio.</t>
+  </si>
+  <si>
+    <t>continous features are word_number_of_syllables, all cells for spanning_tree except constituent_label</t>
+  </si>
+  <si>
+    <t>System</t>
+  </si>
+  <si>
+    <t>BL + syntactic + mention + bigram</t>
+  </si>
+  <si>
+    <t>Logistic</t>
+  </si>
+  <si>
+    <t>BL + syntactic + bigram + pitch accent</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,8 +251,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -178,6 +281,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFBDBD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -204,7 +337,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -215,12 +348,395 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="87">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -382,8 +898,8 @@
   <colors>
     <mruColors>
       <color rgb="FFFFBDBD"/>
+      <color rgb="FF9999FF"/>
       <color rgb="FFFFB9B9"/>
-      <color rgb="FF9999FF"/>
     </mruColors>
   </colors>
   <extLst>
@@ -693,11 +1209,1064 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38E5C8B7-4224-4235-86F8-4913AAEA9BD7}">
+  <dimension ref="A1:Z24"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45:E46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="8.85546875" style="1"/>
+    <col min="4" max="4" width="7.42578125" style="1" customWidth="1"/>
+    <col min="5" max="10" width="8.85546875" style="1"/>
+    <col min="11" max="11" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="1"/>
+    <col min="13" max="14" width="8.85546875" style="1"/>
+    <col min="15" max="15" width="9.140625" style="1"/>
+    <col min="16" max="16384" width="8.85546875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="K2" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="N2" s="2"/>
+      <c r="O2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3"/>
+      <c r="O3" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="P3" s="3">
+        <v>0.38</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>0.49</v>
+      </c>
+      <c r="R3" s="3">
+        <v>0.66800000000000004</v>
+      </c>
+      <c r="S3" s="3">
+        <v>0.73</v>
+      </c>
+      <c r="T3" s="3">
+        <v>0.34</v>
+      </c>
+      <c r="U3" s="3">
+        <v>0.46</v>
+      </c>
+      <c r="V3" s="3">
+        <v>0.67800000000000005</v>
+      </c>
+      <c r="W3" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="X3" s="3">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="Y3" s="3">
+        <v>0.42</v>
+      </c>
+      <c r="Z3" s="3">
+        <v>0.66600000000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="O4" s="3">
+        <v>0.71</v>
+      </c>
+      <c r="P4" s="3">
+        <v>0.42</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>0.53</v>
+      </c>
+      <c r="R4" s="3">
+        <v>0.67400000000000004</v>
+      </c>
+      <c r="S4" s="3">
+        <v>0.72</v>
+      </c>
+      <c r="T4" s="3">
+        <v>0.39</v>
+      </c>
+      <c r="U4" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="V4" s="3">
+        <v>0.68700000000000006</v>
+      </c>
+      <c r="W4" s="3">
+        <v>0.73</v>
+      </c>
+      <c r="X4" s="3">
+        <v>0.32</v>
+      </c>
+      <c r="Y4" s="3">
+        <v>0.45</v>
+      </c>
+      <c r="Z4" s="3">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O5" s="3">
+        <v>0.73</v>
+      </c>
+      <c r="P5" s="3">
+        <v>0.33</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>0.46</v>
+      </c>
+      <c r="R5" s="3">
+        <v>0.68400000000000005</v>
+      </c>
+      <c r="S5" s="3">
+        <v>0.72</v>
+      </c>
+      <c r="T5" s="3">
+        <v>0.39</v>
+      </c>
+      <c r="U5" s="3">
+        <v>0.51</v>
+      </c>
+      <c r="V5" s="3">
+        <v>0.69</v>
+      </c>
+      <c r="W5" s="3">
+        <v>0.73</v>
+      </c>
+      <c r="X5" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="Y5" s="3">
+        <v>0.43</v>
+      </c>
+      <c r="Z5" s="3">
+        <v>0.67600000000000005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O6" s="3">
+        <v>0.72</v>
+      </c>
+      <c r="P6" s="3">
+        <v>0.34</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>0.46</v>
+      </c>
+      <c r="R6" s="3">
+        <v>0.66900000000000004</v>
+      </c>
+      <c r="S6" s="3">
+        <v>0.72</v>
+      </c>
+      <c r="T6" s="3">
+        <v>0.39</v>
+      </c>
+      <c r="U6" s="3">
+        <v>0.51</v>
+      </c>
+      <c r="V6" s="3">
+        <v>0.68700000000000006</v>
+      </c>
+      <c r="W6" s="3">
+        <v>0.72</v>
+      </c>
+      <c r="X6" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="Y6" s="3">
+        <v>0.47</v>
+      </c>
+      <c r="Z6" s="3">
+        <v>0.68400000000000005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O7" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="P7" s="3">
+        <v>0.53</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>0.62</v>
+      </c>
+      <c r="R7" s="3">
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="S7" s="3">
+        <v>0.77</v>
+      </c>
+      <c r="T7" s="3">
+        <v>0.51</v>
+      </c>
+      <c r="U7" s="3">
+        <v>0.62</v>
+      </c>
+      <c r="V7" s="3">
+        <v>0.74099999999999999</v>
+      </c>
+      <c r="W7" s="3">
+        <v>0.79</v>
+      </c>
+      <c r="X7" s="3">
+        <v>0.38</v>
+      </c>
+      <c r="Y7" s="3">
+        <v>0.51</v>
+      </c>
+      <c r="Z7" s="3">
+        <v>0.73399999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O8" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="P8" s="3">
+        <v>0.53</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>0.62</v>
+      </c>
+      <c r="R8" s="3">
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="S8" s="3">
+        <v>0.77</v>
+      </c>
+      <c r="T8" s="3">
+        <v>0.52</v>
+      </c>
+      <c r="U8" s="3">
+        <v>0.62</v>
+      </c>
+      <c r="V8" s="3">
+        <v>0.74</v>
+      </c>
+      <c r="W8" s="3">
+        <v>0.79</v>
+      </c>
+      <c r="X8" s="3">
+        <v>0.39</v>
+      </c>
+      <c r="Y8" s="3">
+        <v>0.52</v>
+      </c>
+      <c r="Z8" s="3">
+        <v>0.73899999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O9" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="P9" s="3">
+        <v>0.53</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>0.62</v>
+      </c>
+      <c r="R9" s="3">
+        <v>0.72799999999999998</v>
+      </c>
+      <c r="S9" s="3">
+        <v>0.76</v>
+      </c>
+      <c r="T9" s="3">
+        <v>0.52</v>
+      </c>
+      <c r="U9" s="3">
+        <v>0.62</v>
+      </c>
+      <c r="V9" s="3">
+        <v>0.73899999999999999</v>
+      </c>
+      <c r="W9" s="3">
+        <v>0.77</v>
+      </c>
+      <c r="X9" s="3">
+        <v>0.44</v>
+      </c>
+      <c r="Y9" s="3">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="Z9" s="3">
+        <v>0.73299999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O10" s="3">
+        <v>0.76</v>
+      </c>
+      <c r="P10" s="3">
+        <v>0.52</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>0.62</v>
+      </c>
+      <c r="R10" s="3">
+        <v>0.74099999999999999</v>
+      </c>
+      <c r="S10" s="3">
+        <v>0.77</v>
+      </c>
+      <c r="T10" s="3">
+        <v>0.52</v>
+      </c>
+      <c r="U10" s="3">
+        <v>0.62</v>
+      </c>
+      <c r="V10" s="3">
+        <v>0.745</v>
+      </c>
+      <c r="W10" s="3">
+        <v>0.87</v>
+      </c>
+      <c r="X10" s="3">
+        <v>0.53</v>
+      </c>
+      <c r="Y10" s="3">
+        <v>0.65</v>
+      </c>
+      <c r="Z10" s="3">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="D11"/>
+      <c r="E11"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
+      <c r="U11" s="3"/>
+      <c r="V11" s="3"/>
+      <c r="W11" s="3"/>
+      <c r="X11" s="3"/>
+      <c r="Y11" s="3"/>
+      <c r="Z11" s="3"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12"/>
+      <c r="E12"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17"/>
+      <c r="E17"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18"/>
+      <c r="E18"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D19"/>
+      <c r="E19"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20"/>
+      <c r="E20"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21"/>
+      <c r="E21"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D22"/>
+      <c r="E22"/>
+    </row>
+    <row r="24" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <conditionalFormatting sqref="L20:L21">
+    <cfRule type="top10" dxfId="86" priority="93" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M20:M21">
+    <cfRule type="top10" dxfId="85" priority="90" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N20:N21">
+    <cfRule type="top10" dxfId="84" priority="87" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J1">
+    <cfRule type="top10" dxfId="83" priority="214" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O1:O11">
+    <cfRule type="top10" dxfId="82" priority="38" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O20:O21">
+    <cfRule type="top10" dxfId="81" priority="39" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O28:O1048576">
+    <cfRule type="top10" dxfId="80" priority="40" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P1:P11">
+    <cfRule type="top10" dxfId="79" priority="35" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P20:P21">
+    <cfRule type="top10" dxfId="78" priority="36" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q1:Q11">
+    <cfRule type="top10" dxfId="77" priority="32" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q20:Q21">
+    <cfRule type="top10" dxfId="76" priority="33" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R1:R11">
+    <cfRule type="top10" dxfId="75" priority="29" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R20:R21">
+    <cfRule type="top10" dxfId="74" priority="30" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S1:S11">
+    <cfRule type="top10" dxfId="73" priority="26" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S20:S21">
+    <cfRule type="top10" dxfId="72" priority="27" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T1:T11">
+    <cfRule type="top10" dxfId="71" priority="23" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T20:T21">
+    <cfRule type="top10" dxfId="70" priority="24" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U1:U11">
+    <cfRule type="top10" dxfId="69" priority="20" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U20:U21">
+    <cfRule type="top10" dxfId="68" priority="21" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V1:V11">
+    <cfRule type="top10" dxfId="67" priority="17" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V20:V21">
+    <cfRule type="top10" dxfId="66" priority="18" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W1:W11">
+    <cfRule type="top10" dxfId="65" priority="14" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W20:W21">
+    <cfRule type="top10" dxfId="64" priority="15" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X1:X11">
+    <cfRule type="top10" dxfId="63" priority="11" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X20:X21">
+    <cfRule type="top10" dxfId="62" priority="12" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y1:Y11">
+    <cfRule type="top10" dxfId="61" priority="8" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y20:Y21">
+    <cfRule type="top10" dxfId="60" priority="9" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z1:Z11">
+    <cfRule type="top10" dxfId="59" priority="5" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z20:Z21">
+    <cfRule type="top10" dxfId="58" priority="6" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L28:L1048576 L22 L12:L19">
+    <cfRule type="top10" dxfId="57" priority="215" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M28:M1048576 M22 M12:M19">
+    <cfRule type="top10" dxfId="56" priority="219" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N28:N1048576 N22 N12:N19">
+    <cfRule type="top10" dxfId="55" priority="223" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O22 O12:O19">
+    <cfRule type="top10" dxfId="54" priority="227" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P28:P1048576 P22 P12:P19">
+    <cfRule type="top10" dxfId="53" priority="231" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q28:Q1048576 Q22 Q12:Q19">
+    <cfRule type="top10" dxfId="52" priority="235" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R28:R1048576 R22 R12:R19">
+    <cfRule type="top10" dxfId="51" priority="239" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S28:S1048576 S22 S12:S19">
+    <cfRule type="top10" dxfId="50" priority="243" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T28:T1048576 T22 T12:T19">
+    <cfRule type="top10" dxfId="49" priority="247" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U28:U1048576 U22 U12:U19">
+    <cfRule type="top10" dxfId="48" priority="251" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V22:V1048576 V12:V19">
+    <cfRule type="top10" dxfId="47" priority="255" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W22:W1048576 W12:W19">
+    <cfRule type="top10" dxfId="46" priority="258" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X22:X1048576 X12:X19">
+    <cfRule type="top10" dxfId="45" priority="261" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y22:Y1048576 Y12:Y19">
+    <cfRule type="top10" dxfId="44" priority="264" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z22:Z1048576 Z12:Z19">
+    <cfRule type="top10" dxfId="43" priority="267" rank="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B23AB93-367B-4549-8B6B-8371BFB65F0E}">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="16">
+        <v>0.7</v>
+      </c>
+      <c r="D2" s="16">
+        <v>0.38</v>
+      </c>
+      <c r="E2" s="16">
+        <v>0.49</v>
+      </c>
+      <c r="F2" s="16">
+        <v>0.66800000000000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="16"/>
+      <c r="B3" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="16">
+        <v>0.73</v>
+      </c>
+      <c r="D3" s="16">
+        <v>0.34</v>
+      </c>
+      <c r="E3" s="16">
+        <v>0.46</v>
+      </c>
+      <c r="F3" s="16">
+        <v>0.67800000000000005</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="16"/>
+      <c r="B4" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="16">
+        <v>0.75</v>
+      </c>
+      <c r="D4" s="16">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="E4" s="16">
+        <v>0.42</v>
+      </c>
+      <c r="F4" s="16">
+        <v>0.66600000000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="16">
+        <v>0.75</v>
+      </c>
+      <c r="D5" s="16">
+        <v>0.53</v>
+      </c>
+      <c r="E5" s="16">
+        <v>0.62</v>
+      </c>
+      <c r="F5" s="16">
+        <v>0.73199999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="16"/>
+      <c r="B6" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="16">
+        <v>0.77</v>
+      </c>
+      <c r="D6" s="16">
+        <v>0.52</v>
+      </c>
+      <c r="E6" s="16">
+        <v>0.62</v>
+      </c>
+      <c r="F6" s="16">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="16"/>
+      <c r="B7" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="16">
+        <v>0.79</v>
+      </c>
+      <c r="D7" s="16">
+        <v>0.39</v>
+      </c>
+      <c r="E7" s="16">
+        <v>0.52</v>
+      </c>
+      <c r="F7" s="16">
+        <v>0.73899999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="18">
+        <v>0.76</v>
+      </c>
+      <c r="D8" s="18">
+        <v>0.52</v>
+      </c>
+      <c r="E8" s="18">
+        <v>0.62</v>
+      </c>
+      <c r="F8" s="18">
+        <v>0.74099999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="18"/>
+      <c r="B9" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="18">
+        <v>0.77</v>
+      </c>
+      <c r="D9" s="18">
+        <v>0.52</v>
+      </c>
+      <c r="E9" s="18">
+        <v>0.62</v>
+      </c>
+      <c r="F9" s="18">
+        <v>0.745</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="18"/>
+      <c r="B10" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="18">
+        <v>0.87</v>
+      </c>
+      <c r="D10" s="18">
+        <v>0.53</v>
+      </c>
+      <c r="E10" s="18">
+        <v>0.65</v>
+      </c>
+      <c r="F10" s="18">
+        <v>0.82</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B3">
+    <cfRule type="top10" dxfId="42" priority="6" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4">
+    <cfRule type="top10" dxfId="41" priority="5" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6">
+    <cfRule type="top10" dxfId="40" priority="4" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7">
+    <cfRule type="top10" dxfId="39" priority="3" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9">
+    <cfRule type="top10" dxfId="1" priority="2" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B10">
+    <cfRule type="top10" dxfId="0" priority="1" rank="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E3431B5-E431-4926-B262-9A69677D0E6D}">
   <dimension ref="A1:AC20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+      <selection activeCell="V1" sqref="V1:V1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1566,63 +3135,63 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="W12 T14:T15">
-    <cfRule type="top10" dxfId="25" priority="19" rank="1"/>
+    <cfRule type="top10" dxfId="26" priority="19" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P14">
-    <cfRule type="top10" dxfId="24" priority="14" rank="1"/>
+    <cfRule type="top10" dxfId="25" priority="14" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC2">
-    <cfRule type="top10" dxfId="23" priority="9" rank="1"/>
+    <cfRule type="top10" dxfId="24" priority="9" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB2">
-    <cfRule type="top10" dxfId="22" priority="7" rank="1"/>
+    <cfRule type="top10" dxfId="23" priority="7" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB5">
-    <cfRule type="top10" dxfId="21" priority="5" rank="1"/>
+    <cfRule type="top10" dxfId="22" priority="5" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA2">
-    <cfRule type="top10" dxfId="20" priority="3" rank="1"/>
+    <cfRule type="top10" dxfId="21" priority="3" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA5">
-    <cfRule type="top10" dxfId="19" priority="2" rank="1"/>
+    <cfRule type="top10" dxfId="20" priority="2" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="X14:X15 AA12:AA13">
-    <cfRule type="top10" dxfId="18" priority="33" rank="1"/>
+    <cfRule type="top10" dxfId="19" priority="33" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z1:Z1048576">
-    <cfRule type="top10" dxfId="17" priority="1" rank="1"/>
+    <cfRule type="top10" dxfId="18" priority="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q14:Q15 T12:T13 W1:W11">
-    <cfRule type="top10" dxfId="16" priority="34" rank="1"/>
+    <cfRule type="top10" dxfId="17" priority="34" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R14:R15 U12:U13 X1:X11">
-    <cfRule type="top10" dxfId="15" priority="38" rank="1"/>
+    <cfRule type="top10" dxfId="16" priority="38" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="S12:S13 P15 V1:V11">
-    <cfRule type="top10" dxfId="14" priority="42" rank="1"/>
+    <cfRule type="top10" dxfId="15" priority="42" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="S14:S1048576 V12:V13 Y1:Y11">
-    <cfRule type="top10" dxfId="13" priority="46" rank="1"/>
+    <cfRule type="top10" dxfId="14" priority="46" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="W14:W1048576 AC1 AC3:AC11">
-    <cfRule type="top10" dxfId="12" priority="50" rank="1"/>
+    <cfRule type="top10" dxfId="13" priority="50" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V14:V1048576 AB1 AB3:AB4 Y12:Y13 AB6:AB11">
-    <cfRule type="top10" dxfId="11" priority="54" rank="1"/>
+    <cfRule type="top10" dxfId="12" priority="54" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U14:U1048576 AA1 AA3:AA4 X12:X13 AA6:AA11">
-    <cfRule type="top10" dxfId="10" priority="60" rank="1"/>
+    <cfRule type="top10" dxfId="11" priority="60" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D8B1718-FE79-4AC3-B485-AAA055742648}">
   <dimension ref="A1:X16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O2" workbookViewId="0">
-      <selection activeCell="Y17" sqref="Y17"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2277,31 +3846,31 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="R1:R1048576">
-    <cfRule type="top10" dxfId="9" priority="14" rank="1"/>
+    <cfRule type="top10" dxfId="10" priority="14" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V3:V13">
-    <cfRule type="top10" dxfId="7" priority="8" rank="1"/>
+    <cfRule type="top10" dxfId="9" priority="8" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V14:V1048576 W1:W13 W15">
-    <cfRule type="top10" dxfId="6" priority="7" rank="1"/>
+    <cfRule type="top10" dxfId="8" priority="7" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:U13 U15">
-    <cfRule type="top10" dxfId="5" priority="6" rank="1"/>
+    <cfRule type="top10" dxfId="7" priority="6" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q14">
-    <cfRule type="top10" dxfId="4" priority="4" rank="1"/>
+    <cfRule type="top10" dxfId="6" priority="4" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q15:Q1048576 Q1:Q13">
-    <cfRule type="top10" dxfId="3" priority="16" rank="1"/>
+    <cfRule type="top10" dxfId="5" priority="16" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1:S1048576">
-    <cfRule type="top10" dxfId="2" priority="3" rank="1"/>
+    <cfRule type="top10" dxfId="4" priority="3" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1:T1048576">
-    <cfRule type="top10" dxfId="1" priority="2" rank="1"/>
+    <cfRule type="top10" dxfId="3" priority="2" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="X1:X13 X15">
-    <cfRule type="top10" dxfId="0" priority="1" rank="1"/>
+    <cfRule type="top10" dxfId="2" priority="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>